<commit_message>
test case for download client gst info
</commit_message>
<xml_diff>
--- a/bpg-cbt-apac-services-api-test-suite/acceptance-test/client_gst_info/resources/add_client_gst__info.xlsx
+++ b/bpg-cbt-apac-services-api-test-suite/acceptance-test/client_gst_info/resources/add_client_gst__info.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Free Format</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>191 Yerwada</t>
-  </si>
-  <si>
-    <t>411 006</t>
   </si>
   <si>
     <t>Pune</t>
@@ -1601,8 +1598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1693,7 +1690,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>20</v>
@@ -1726,7 +1723,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>27</v>
@@ -1743,11 +1740,11 @@
       <c r="G4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>31</v>
+      <c r="H4" s="5">
+        <v>411006</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>25</v>
@@ -1756,100 +1753,100 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="7">
         <v>912266003000</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="G5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H5" s="5">
         <v>122002</v>
       </c>
       <c r="I5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="K5" s="30"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="7">
         <v>912266003000</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="5">
         <v>110037</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="7">
         <v>912266003000</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H7" s="5">
         <v>201301</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" s="30"/>
     </row>

</xml_diff>